<commit_message>
controller rev.30 (interrupts for echo)
</commit_message>
<xml_diff>
--- a/docs/Calibration_test.xlsx
+++ b/docs/Calibration_test.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\arhive\lena\arduino\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="9345" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="9345" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -17,13 +12,15 @@
     <sheet name="Chart (norm)" sheetId="2" r:id="rId3"/>
     <sheet name="SIN_COS" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="FIgure1" sheetId="7" r:id="rId6"/>
+    <sheet name="Figure2" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>Power</t>
   </si>
@@ -210,12 +207,33 @@
   <si>
     <t>correction</t>
   </si>
+  <si>
+    <t>Move 0°</t>
+  </si>
+  <si>
+    <t>Move 45°</t>
+  </si>
+  <si>
+    <t>Move 15°</t>
+  </si>
+  <si>
+    <t>Move 30°</t>
+  </si>
+  <si>
+    <t>Turning (Kt)</t>
+  </si>
+  <si>
+    <t>Rotation (Kr)</t>
+  </si>
+  <si>
+    <t>Rotate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +245,15 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -283,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -299,6 +326,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3453,11 +3481,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="191919664"/>
-        <c:axId val="192045344"/>
+        <c:axId val="83517824"/>
+        <c:axId val="83519360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="191919664"/>
+        <c:axId val="83517824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260"/>
@@ -3471,12 +3499,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="192045344"/>
+        <c:crossAx val="83519360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="192045344"/>
+        <c:axId val="83519360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3488,7 +3516,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191919664"/>
+        <c:crossAx val="83517824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5747,11 +5775,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="192238936"/>
-        <c:axId val="192197856"/>
+        <c:axId val="83615104"/>
+        <c:axId val="83620992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="192238936"/>
+        <c:axId val="83615104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260"/>
@@ -5765,12 +5793,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="192197856"/>
+        <c:crossAx val="83620992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="192197856"/>
+        <c:axId val="83620992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5782,7 +5810,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="192238936"/>
+        <c:crossAx val="83615104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6076,11 +6104,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="192953936"/>
-        <c:axId val="192067864"/>
+        <c:axId val="84821888"/>
+        <c:axId val="84836352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="192953936"/>
+        <c:axId val="84821888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6137,12 +6165,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192067864"/>
+        <c:crossAx val="84836352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="192067864"/>
+        <c:axId val="84836352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6199,7 +6227,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192953936"/>
+        <c:crossAx val="84821888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6240,6 +6268,2318 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>FIgure1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rotate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>FIgure1!$A$2:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9215686274509803E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.8431372549019607E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11764705882352941</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15686274509803921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19607843137254902</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23529411764705882</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.27450980392156865</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.31372549019607843</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.35294117647058826</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.39215686274509803</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.43137254901960786</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.47058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.50980392156862742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5490196078431373</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.58823529411764708</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.62745098039215685</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.70588235294117652</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.74509803921568629</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.78431372549019607</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.82352941176470584</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.86274509803921573</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.90196078431372551</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.94117647058823528</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98039215686274506</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>FIgure1!$D$2:$D$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="6">
+                  <c:v>23.881188118811881</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31.736842105263158</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.6875</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43.071428571428569</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>49.224489795918366</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>53.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>59.117647058823522</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65.189189189189193</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70.116279069767444</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75.375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>84.335664335664333</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>94.21875</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>99.669421487603302</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>104.41558441558441</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>109.14027149321267</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>114.85714285714286</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>118.81773399014779</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>124.32989690721649</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>127.61904761904762</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>FIgure1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Move 0°</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>FIgure1!$A$2:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9215686274509803E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.8431372549019607E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11764705882352941</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15686274509803921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19607843137254902</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23529411764705882</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.27450980392156865</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.31372549019607843</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.35294117647058826</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.39215686274509803</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.43137254901960786</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.47058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.50980392156862742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5490196078431373</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.58823529411764708</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.62745098039215685</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.70588235294117652</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.74509803921568629</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.78431372549019607</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.82352941176470584</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.86274509803921573</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.90196078431372551</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.94117647058823528</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98039215686274506</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>FIgure1!$B$2:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>109</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>FIgure1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Move 45°</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>FIgure1!$A$2:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9215686274509803E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.8431372549019607E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11764705882352941</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15686274509803921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19607843137254902</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23529411764705882</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.27450980392156865</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.31372549019607843</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.35294117647058826</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.39215686274509803</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.43137254901960786</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.47058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.50980392156862742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5490196078431373</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.58823529411764708</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.62745098039215685</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.70588235294117652</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.74509803921568629</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.78431372549019607</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.82352941176470584</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.86274509803921573</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.90196078431372551</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.94117647058823528</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98039215686274506</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>FIgure1!$C$2:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="38617472"/>
+        <c:axId val="38570624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="38617472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="38570624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="38570624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="140"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="38617472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.84477050424442668"/>
+          <c:y val="0.67382380422482957"/>
+          <c:w val="0.12690827845730704"/>
+          <c:h val="0.21764756149667339"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Figure2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Turning (Kt)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Figure2!$A$2:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9215686274509803E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.8431372549019607E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11764705882352941</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15686274509803921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19607843137254902</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23529411764705882</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.27450980392156865</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.31372549019607843</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.35294117647058826</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.39215686274509803</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.43137254901960786</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.47058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.50980392156862742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5490196078431373</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.58823529411764708</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.62745098039215685</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.70588235294117652</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.74509803921568629</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.78431372549019607</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.82352941176470584</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.86274509803921573</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.90196078431372551</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.94117647058823528</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98039215686274506</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Figure2!$B$2:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.27450980392156865</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29803921568627451</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.32156862745098042</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34509803921568627</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.36862745098039218</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.39215686274509803</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.47058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5490196078431373</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.62745098039215685</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.70588235294117652</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.78431372549019607</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.86274509803921573</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.94117647058823528</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0196078431372548</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0980392156862746</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.1764705882352942</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.2549019607843137</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.3333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.411764705882353</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.4901960784313726</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.5686274509803921</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.6470588235294117</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.7254901960784315</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.803921568627451</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.8823529411764706</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.9607843137254901</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Figure2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rotation (Kr)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Figure2!$A$2:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9215686274509803E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.8431372549019607E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11764705882352941</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15686274509803921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19607843137254902</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23529411764705882</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.27450980392156865</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.31372549019607843</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.35294117647058826</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.39215686274509803</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.43137254901960786</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.47058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.50980392156862742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5490196078431373</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.58823529411764708</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.62745098039215685</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.70588235294117652</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.74509803921568629</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.78431372549019607</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.82352941176470584</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.86274509803921573</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.90196078431372551</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.94117647058823528</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98039215686274506</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Figure2!$C$2:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.30117647058823532</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.37019418566823414</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43921190074823296</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.50822961582823178</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.57724733090823055</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.64626504598822931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71528276106822819</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.79742868127643207</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.89270280661284118</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98797693194925018</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0832510572856593</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1785251826220684</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2737993079584775</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3690734332948866</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4643475586312955</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5596216839677046</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.654895809304114</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7501699346405226</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8454440599769319</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9407181853133408</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.0359923106497497</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1312664359861593</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2265405613225684</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.3218146866589771</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4170888119953866</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5123629373317953</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="74273152"/>
+        <c:axId val="74275072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="74273152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="74275072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="74275072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="74273152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.80601515425732551"/>
+          <c:y val="0.63804562891177052"/>
+          <c:w val="0.16446481819374717"/>
+          <c:h val="0.10933322064616699"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Figure2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Move 0°</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Figure2!$A$2:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9215686274509803E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.8431372549019607E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11764705882352941</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15686274509803921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19607843137254902</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23529411764705882</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.27450980392156865</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.31372549019607843</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.35294117647058826</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.39215686274509803</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.43137254901960786</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.47058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.50980392156862742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5490196078431373</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.58823529411764708</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.62745098039215685</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.70588235294117652</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.74509803921568629</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.78431372549019607</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.82352941176470584</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.86274509803921573</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.90196078431372551</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.94117647058823528</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98039215686274506</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Figure2!$D$2:$D$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.47058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52887351018838913</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.58715878508266051</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.64544405997693199</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70372933487120337</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.76201460976547486</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.82029988465974624</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.87858515955401773</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9368704344482891</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99515570934256048</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.053440984236832</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1117262591311035</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1700115340253749</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2282968089196462</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2865820838139179</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.344867358708189</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.4031526336024607</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4614379084967322</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5197231833910034</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.5780084582852749</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.6362937331795464</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.7024221453287198</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.7685505574778932</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.8346789696270667</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.9008073817762399</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.9669357939254133</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Figure2!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Move 15°</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="lgDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Figure2!$A$2:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9215686274509803E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.8431372549019607E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11764705882352941</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15686274509803921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19607843137254902</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23529411764705882</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.27450980392156865</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.31372549019607843</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.35294117647058826</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.39215686274509803</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.43137254901960786</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.47058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.50980392156862742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5490196078431373</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.58823529411764708</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.62745098039215685</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.70588235294117652</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.74509803921568629</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.78431372549019607</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.82352941176470584</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.86274509803921573</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.90196078431372551</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.94117647058823528</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98039215686274506</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Figure2!$F$2:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.55529411764705883</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.62407074202229917</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69284736639753941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76162399077277976</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83040061514801988</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89917723952326034</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.96795386389850047</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0367304882737409</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.105507112648981</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1742837370242214</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2430603613994617</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.3118369857747021</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3806136101499424</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4493902345251823</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5181668589004231</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5869434832756628</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6557201076509036</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.724496732026144</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.7932733564013839</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.8620499807766242</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.9308266051518646</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.0088581314878895</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.0868896578239138</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.1649211841599385</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.2429527104959628</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.3209842368319875</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Figure2!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Move 30°</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Figure2!$A$2:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9215686274509803E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.8431372549019607E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11764705882352941</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15686274509803921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19607843137254902</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23529411764705882</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.27450980392156865</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.31372549019607843</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.35294117647058826</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.39215686274509803</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.43137254901960786</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.47058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.50980392156862742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5490196078431373</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.58823529411764708</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.62745098039215685</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.70588235294117652</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.74509803921568629</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.78431372549019607</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.82352941176470584</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.86274509803921573</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.90196078431372551</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.94117647058823528</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98039215686274506</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Figure2!$G$2:$G$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.64941176470588224</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72984544405997698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.81027912341407149</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89071280276816611</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97114648212226062</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0515801614763551</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1320138408304496</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2124475201845444</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2928811995386389</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3733148788927334</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4537485582468279</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5341822376009226</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6146159169550174</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.6950495963091117</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.7754832756632066</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.8559169550173007</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.9363506343713957</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.0167843137254904</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.0972179930795845</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.1776516724336794</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.2580853517877739</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.3493425605536333</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.4405997693194923</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.5318569780853517</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.6231141868512107</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.7143713956170701</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Figure2!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Move 45°</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Figure2!$A$2:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9215686274509803E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.8431372549019607E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11764705882352941</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15686274509803921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19607843137254902</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23529411764705882</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.27450980392156865</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.31372549019607843</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.35294117647058826</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.39215686274509803</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.43137254901960786</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.47058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.50980392156862742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5490196078431373</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.58823529411764708</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.62745098039215685</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.70588235294117652</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.74509803921568629</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.78431372549019607</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.82352941176470584</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.86274509803921573</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.90196078431372551</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.94117647058823528</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98039215686274506</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Figure2!$E$2:$E$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.73411764705882354</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82504267589388702</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91596770472895039</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0068927335640139</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0978177623990772</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1887427912341408</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2796678200692042</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3705928489042678</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.461517877739331</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5524429065743943</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6433679354094579</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.7342929642445215</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.8252179930795849</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9161430219146482</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0070680507497118</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.097993079584775</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1889181084198386</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.2798431372549022</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.3707681660899653</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.4616931949250289</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.5526182237600925</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.6557785467128032</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.7589388696655135</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.8620991926182242</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.9652595155709345</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.0684198385236447</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="73872896"/>
+        <c:axId val="73874432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="73872896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="73874432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="73874432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3.5"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="73872896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.82131530164971966"/>
+          <c:y val="0.68088046239300593"/>
+          <c:w val="0.13749992077570794"/>
+          <c:h val="0.21866644129233398"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -6913,6 +9253,110 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>14286</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>604839</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>604839</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6956,7 +9400,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6991,7 +9435,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7203,8 +9647,8 @@
   <dimension ref="A1:AO50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L14" sqref="L14"/>
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7236,7 +9680,7 @@
     <col min="27" max="27" width="9.85546875" customWidth="1"/>
     <col min="28" max="28" width="10.5703125" style="10" customWidth="1"/>
     <col min="29" max="29" width="16.85546875" customWidth="1"/>
-    <col min="30" max="30" width="8.85546875" customWidth="1"/>
+    <col min="30" max="30" width="10.140625" customWidth="1"/>
     <col min="31" max="31" width="9.28515625" customWidth="1"/>
     <col min="34" max="34" width="12.140625" customWidth="1"/>
     <col min="35" max="35" width="9.140625" style="10"/>
@@ -10765,7 +13209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="X32" sqref="X32"/>
     </sheetView>
   </sheetViews>
@@ -10783,7 +13227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
@@ -12523,4 +14967,1299 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>Data!A2/255</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <f>Data!A3/255</f>
+        <v>3.9215686274509803E-2</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <f>Data!A4/255</f>
+        <v>7.8431372549019607E-2</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <f>Data!A5/255</f>
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <f>Data!A6/255</f>
+        <v>0.15686274509803921</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <f>Data!A7/255</f>
+        <v>0.19607843137254902</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <f>Data!A8/255</f>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10">
+        <f>Data!AA8/10</f>
+        <v>23.881188118811881</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <f>Data!A9/255</f>
+        <v>0.27450980392156865</v>
+      </c>
+      <c r="B9" s="10">
+        <f>Data!B9/10</f>
+        <v>12</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10">
+        <f>Data!AA9/10</f>
+        <v>31.736842105263158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <f>Data!A10/255</f>
+        <v>0.31372549019607843</v>
+      </c>
+      <c r="B10" s="10">
+        <f>Data!B10/10</f>
+        <v>19</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10">
+        <f>Data!AA10/10</f>
+        <v>37.6875</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <f>Data!A11/255</f>
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="B11" s="10">
+        <f>Data!B11/10</f>
+        <v>28</v>
+      </c>
+      <c r="C11" s="10">
+        <f>Data!N11/10</f>
+        <v>13</v>
+      </c>
+      <c r="D11" s="10">
+        <f>Data!AA11/10</f>
+        <v>43.071428571428569</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <f>Data!A12/255</f>
+        <v>0.39215686274509803</v>
+      </c>
+      <c r="B12" s="10">
+        <f>Data!B12/10</f>
+        <v>35</v>
+      </c>
+      <c r="C12" s="10">
+        <f>Data!N12/10</f>
+        <v>21</v>
+      </c>
+      <c r="D12" s="10">
+        <f>Data!AA12/10</f>
+        <v>49.224489795918366</v>
+      </c>
+      <c r="W12" s="15"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <f>Data!A13/255</f>
+        <v>0.43137254901960786</v>
+      </c>
+      <c r="B13" s="10">
+        <f>Data!B13/10</f>
+        <v>42</v>
+      </c>
+      <c r="C13" s="10">
+        <f>Data!N13/10</f>
+        <v>28</v>
+      </c>
+      <c r="D13" s="10">
+        <f>Data!AA13/10</f>
+        <v>53.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <f>Data!A14/255</f>
+        <v>0.47058823529411764</v>
+      </c>
+      <c r="B14" s="10">
+        <f>Data!B14/10</f>
+        <v>48</v>
+      </c>
+      <c r="C14" s="10">
+        <f>Data!N14/10</f>
+        <v>36</v>
+      </c>
+      <c r="D14" s="10">
+        <f>Data!AA14/10</f>
+        <v>59.117647058823522</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <f>Data!A15/255</f>
+        <v>0.50980392156862742</v>
+      </c>
+      <c r="B15" s="10">
+        <f>Data!B15/10</f>
+        <v>53</v>
+      </c>
+      <c r="C15" s="10">
+        <f>Data!N15/10</f>
+        <v>40</v>
+      </c>
+      <c r="D15" s="10">
+        <f>Data!AA15/10</f>
+        <v>65.189189189189193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <f>Data!A16/255</f>
+        <v>0.5490196078431373</v>
+      </c>
+      <c r="B16" s="10">
+        <f>Data!B16/10</f>
+        <v>57</v>
+      </c>
+      <c r="C16" s="10">
+        <f>Data!N16/10</f>
+        <v>46</v>
+      </c>
+      <c r="D16" s="10">
+        <f>Data!AA16/10</f>
+        <v>70.116279069767444</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <f>Data!A17/255</f>
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="B17" s="10">
+        <f>Data!B17/10</f>
+        <v>62</v>
+      </c>
+      <c r="C17" s="10">
+        <f>Data!N17/10</f>
+        <v>49</v>
+      </c>
+      <c r="D17" s="10">
+        <f>Data!AA17/10</f>
+        <v>75.375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <f>Data!A18/255</f>
+        <v>0.62745098039215685</v>
+      </c>
+      <c r="B18" s="10">
+        <f>Data!B18/10</f>
+        <v>66</v>
+      </c>
+      <c r="C18" s="10">
+        <f>Data!N18/10</f>
+        <v>55</v>
+      </c>
+      <c r="D18" s="10">
+        <f>Data!AA18/10</f>
+        <v>80.400000000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <f>Data!A19/255</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B19" s="10">
+        <f>Data!B19/10</f>
+        <v>71</v>
+      </c>
+      <c r="C19" s="10">
+        <f>Data!N19/10</f>
+        <v>59</v>
+      </c>
+      <c r="D19" s="10">
+        <f>Data!AA19/10</f>
+        <v>84.335664335664333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <f>Data!A20/255</f>
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="B20" s="10">
+        <f>Data!B20/10</f>
+        <v>75</v>
+      </c>
+      <c r="C20" s="10">
+        <f>Data!N20/10</f>
+        <v>63</v>
+      </c>
+      <c r="D20" s="10">
+        <f>Data!AA20/10</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <f>Data!A21/255</f>
+        <v>0.74509803921568629</v>
+      </c>
+      <c r="B21" s="10">
+        <f>Data!B21/10</f>
+        <v>79</v>
+      </c>
+      <c r="C21" s="10">
+        <f>Data!N21/10</f>
+        <v>70</v>
+      </c>
+      <c r="D21" s="10">
+        <f>Data!AA21/10</f>
+        <v>94.21875</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <f>Data!A22/255</f>
+        <v>0.78431372549019607</v>
+      </c>
+      <c r="B22" s="10">
+        <f>Data!B22/10</f>
+        <v>85</v>
+      </c>
+      <c r="C22" s="10">
+        <f>Data!N22/10</f>
+        <v>76</v>
+      </c>
+      <c r="D22" s="10">
+        <f>Data!AA22/10</f>
+        <v>99.669421487603302</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <f>Data!A23/255</f>
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="B23" s="10">
+        <f>Data!B23/10</f>
+        <v>88</v>
+      </c>
+      <c r="C23" s="10">
+        <f>Data!N23/10</f>
+        <v>81</v>
+      </c>
+      <c r="D23" s="10">
+        <f>Data!AA23/10</f>
+        <v>104.41558441558441</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <f>Data!A24/255</f>
+        <v>0.86274509803921573</v>
+      </c>
+      <c r="B24" s="10">
+        <f>Data!B24/10</f>
+        <v>93</v>
+      </c>
+      <c r="C24" s="10">
+        <f>Data!N24/10</f>
+        <v>83</v>
+      </c>
+      <c r="D24" s="10">
+        <f>Data!AA24/10</f>
+        <v>109.14027149321267</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <f>Data!A25/255</f>
+        <v>0.90196078431372551</v>
+      </c>
+      <c r="B25" s="10">
+        <f>Data!B25/10</f>
+        <v>97</v>
+      </c>
+      <c r="C25" s="10">
+        <f>Data!N25/10</f>
+        <v>89</v>
+      </c>
+      <c r="D25" s="10">
+        <f>Data!AA25/10</f>
+        <v>114.85714285714286</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <f>Data!A26/255</f>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="B26" s="10">
+        <f>Data!B26/10</f>
+        <v>102</v>
+      </c>
+      <c r="C26" s="10">
+        <f>Data!N26/10</f>
+        <v>93</v>
+      </c>
+      <c r="D26" s="10">
+        <f>Data!AA26/10</f>
+        <v>118.81773399014779</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <f>Data!A27/255</f>
+        <v>0.98039215686274506</v>
+      </c>
+      <c r="B27" s="10">
+        <f>Data!B27/10</f>
+        <v>106</v>
+      </c>
+      <c r="C27" s="10">
+        <f>Data!N27/10</f>
+        <v>93</v>
+      </c>
+      <c r="D27" s="10">
+        <f>Data!AA27/10</f>
+        <v>124.32989690721649</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <f>Data!A28/255</f>
+        <v>1</v>
+      </c>
+      <c r="B28" s="10">
+        <f>Data!B28/10</f>
+        <v>109</v>
+      </c>
+      <c r="C28" s="10">
+        <f>Data!N28/10</f>
+        <v>99</v>
+      </c>
+      <c r="D28" s="10">
+        <f>Data!AA28/10</f>
+        <v>127.61904761904762</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <f>Data!A2/255</f>
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>Data!AD2/255*2</f>
+        <v>0.27450980392156865</v>
+      </c>
+      <c r="C2">
+        <f>Data!AE2/255*2.56</f>
+        <v>0.30117647058823532</v>
+      </c>
+      <c r="D2">
+        <f>Data!L2/255*2</f>
+        <v>0.47058823529411764</v>
+      </c>
+      <c r="E2">
+        <f>Data!L2/255*2*1.56</f>
+        <v>0.73411764705882354</v>
+      </c>
+      <c r="F2">
+        <f>Data!L2/255*2*1.18</f>
+        <v>0.55529411764705883</v>
+      </c>
+      <c r="G2">
+        <f>Data!L2/255*2*1.38</f>
+        <v>0.64941176470588224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <f>Data!A3/255</f>
+        <v>3.9215686274509803E-2</v>
+      </c>
+      <c r="B3" s="10">
+        <f>Data!AD3/255*2</f>
+        <v>0.29803921568627451</v>
+      </c>
+      <c r="C3" s="10">
+        <f>Data!AE3/255*2.56</f>
+        <v>0.37019418566823414</v>
+      </c>
+      <c r="D3" s="10">
+        <f>Data!L3/255*2</f>
+        <v>0.52887351018838913</v>
+      </c>
+      <c r="E3" s="10">
+        <f>Data!L3/255*2*1.56</f>
+        <v>0.82504267589388702</v>
+      </c>
+      <c r="F3" s="10">
+        <f>Data!L3/255*2*1.18</f>
+        <v>0.62407074202229917</v>
+      </c>
+      <c r="G3" s="10">
+        <f>Data!L3/255*2*1.38</f>
+        <v>0.72984544405997698</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <f>Data!A4/255</f>
+        <v>7.8431372549019607E-2</v>
+      </c>
+      <c r="B4" s="10">
+        <f>Data!AD4/255*2</f>
+        <v>0.32156862745098042</v>
+      </c>
+      <c r="C4" s="10">
+        <f>Data!AE4/255*2.56</f>
+        <v>0.43921190074823296</v>
+      </c>
+      <c r="D4" s="10">
+        <f>Data!L4/255*2</f>
+        <v>0.58715878508266051</v>
+      </c>
+      <c r="E4" s="10">
+        <f>Data!L4/255*2*1.56</f>
+        <v>0.91596770472895039</v>
+      </c>
+      <c r="F4" s="10">
+        <f>Data!L4/255*2*1.18</f>
+        <v>0.69284736639753941</v>
+      </c>
+      <c r="G4" s="10">
+        <f>Data!L4/255*2*1.38</f>
+        <v>0.81027912341407149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <f>Data!A5/255</f>
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="B5" s="10">
+        <f>Data!AD5/255*2</f>
+        <v>0.34509803921568627</v>
+      </c>
+      <c r="C5" s="10">
+        <f>Data!AE5/255*2.56</f>
+        <v>0.50822961582823178</v>
+      </c>
+      <c r="D5" s="10">
+        <f>Data!L5/255*2</f>
+        <v>0.64544405997693199</v>
+      </c>
+      <c r="E5" s="10">
+        <f>Data!L5/255*2*1.56</f>
+        <v>1.0068927335640139</v>
+      </c>
+      <c r="F5" s="10">
+        <f>Data!L5/255*2*1.18</f>
+        <v>0.76162399077277976</v>
+      </c>
+      <c r="G5" s="10">
+        <f>Data!L5/255*2*1.38</f>
+        <v>0.89071280276816611</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <f>Data!A6/255</f>
+        <v>0.15686274509803921</v>
+      </c>
+      <c r="B6" s="10">
+        <f>Data!AD6/255*2</f>
+        <v>0.36862745098039218</v>
+      </c>
+      <c r="C6" s="10">
+        <f>Data!AE6/255*2.56</f>
+        <v>0.57724733090823055</v>
+      </c>
+      <c r="D6" s="10">
+        <f>Data!L6/255*2</f>
+        <v>0.70372933487120337</v>
+      </c>
+      <c r="E6" s="10">
+        <f>Data!L6/255*2*1.56</f>
+        <v>1.0978177623990772</v>
+      </c>
+      <c r="F6" s="10">
+        <f>Data!L6/255*2*1.18</f>
+        <v>0.83040061514801988</v>
+      </c>
+      <c r="G6" s="10">
+        <f>Data!L6/255*2*1.38</f>
+        <v>0.97114648212226062</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <f>Data!A7/255</f>
+        <v>0.19607843137254902</v>
+      </c>
+      <c r="B7" s="10">
+        <f>Data!AD7/255*2</f>
+        <v>0.39215686274509803</v>
+      </c>
+      <c r="C7" s="10">
+        <f>Data!AE7/255*2.56</f>
+        <v>0.64626504598822931</v>
+      </c>
+      <c r="D7" s="10">
+        <f>Data!L7/255*2</f>
+        <v>0.76201460976547486</v>
+      </c>
+      <c r="E7" s="10">
+        <f>Data!L7/255*2*1.56</f>
+        <v>1.1887427912341408</v>
+      </c>
+      <c r="F7" s="10">
+        <f>Data!L7/255*2*1.18</f>
+        <v>0.89917723952326034</v>
+      </c>
+      <c r="G7" s="10">
+        <f>Data!L7/255*2*1.38</f>
+        <v>1.0515801614763551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <f>Data!A8/255</f>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="B8" s="10">
+        <f>Data!AD8/255*2</f>
+        <v>0.47058823529411764</v>
+      </c>
+      <c r="C8" s="10">
+        <f>Data!AE8/255*2.56</f>
+        <v>0.71528276106822819</v>
+      </c>
+      <c r="D8" s="10">
+        <f>Data!L8/255*2</f>
+        <v>0.82029988465974624</v>
+      </c>
+      <c r="E8" s="10">
+        <f>Data!L8/255*2*1.56</f>
+        <v>1.2796678200692042</v>
+      </c>
+      <c r="F8" s="10">
+        <f>Data!L8/255*2*1.18</f>
+        <v>0.96795386389850047</v>
+      </c>
+      <c r="G8" s="10">
+        <f>Data!L8/255*2*1.38</f>
+        <v>1.1320138408304496</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <f>Data!A9/255</f>
+        <v>0.27450980392156865</v>
+      </c>
+      <c r="B9" s="10">
+        <f>Data!AD9/255*2</f>
+        <v>0.5490196078431373</v>
+      </c>
+      <c r="C9" s="10">
+        <f>Data!AE9/255*2.56</f>
+        <v>0.79742868127643207</v>
+      </c>
+      <c r="D9" s="10">
+        <f>Data!L9/255*2</f>
+        <v>0.87858515955401773</v>
+      </c>
+      <c r="E9" s="10">
+        <f>Data!L9/255*2*1.56</f>
+        <v>1.3705928489042678</v>
+      </c>
+      <c r="F9" s="10">
+        <f>Data!L9/255*2*1.18</f>
+        <v>1.0367304882737409</v>
+      </c>
+      <c r="G9" s="10">
+        <f>Data!L9/255*2*1.38</f>
+        <v>1.2124475201845444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <f>Data!A10/255</f>
+        <v>0.31372549019607843</v>
+      </c>
+      <c r="B10" s="10">
+        <f>Data!AD10/255*2</f>
+        <v>0.62745098039215685</v>
+      </c>
+      <c r="C10" s="10">
+        <f>Data!AE10/255*2.56</f>
+        <v>0.89270280661284118</v>
+      </c>
+      <c r="D10" s="10">
+        <f>Data!L10/255*2</f>
+        <v>0.9368704344482891</v>
+      </c>
+      <c r="E10" s="10">
+        <f>Data!L10/255*2*1.56</f>
+        <v>1.461517877739331</v>
+      </c>
+      <c r="F10" s="10">
+        <f>Data!L10/255*2*1.18</f>
+        <v>1.105507112648981</v>
+      </c>
+      <c r="G10" s="10">
+        <f>Data!L10/255*2*1.38</f>
+        <v>1.2928811995386389</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <f>Data!A11/255</f>
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="B11" s="10">
+        <f>Data!AD11/255*2</f>
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="C11" s="10">
+        <f>Data!AE11/255*2.56</f>
+        <v>0.98797693194925018</v>
+      </c>
+      <c r="D11" s="10">
+        <f>Data!L11/255*2</f>
+        <v>0.99515570934256048</v>
+      </c>
+      <c r="E11" s="10">
+        <f>Data!L11/255*2*1.56</f>
+        <v>1.5524429065743943</v>
+      </c>
+      <c r="F11" s="10">
+        <f>Data!L11/255*2*1.18</f>
+        <v>1.1742837370242214</v>
+      </c>
+      <c r="G11" s="10">
+        <f>Data!L11/255*2*1.38</f>
+        <v>1.3733148788927334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <f>Data!A12/255</f>
+        <v>0.39215686274509803</v>
+      </c>
+      <c r="B12" s="10">
+        <f>Data!AD12/255*2</f>
+        <v>0.78431372549019607</v>
+      </c>
+      <c r="C12" s="10">
+        <f>Data!AE12/255*2.56</f>
+        <v>1.0832510572856593</v>
+      </c>
+      <c r="D12" s="10">
+        <f>Data!L12/255*2</f>
+        <v>1.053440984236832</v>
+      </c>
+      <c r="E12" s="10">
+        <f>Data!L12/255*2*1.56</f>
+        <v>1.6433679354094579</v>
+      </c>
+      <c r="F12" s="10">
+        <f>Data!L12/255*2*1.18</f>
+        <v>1.2430603613994617</v>
+      </c>
+      <c r="G12" s="10">
+        <f>Data!L12/255*2*1.38</f>
+        <v>1.4537485582468279</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <f>Data!A13/255</f>
+        <v>0.43137254901960786</v>
+      </c>
+      <c r="B13" s="10">
+        <f>Data!AD13/255*2</f>
+        <v>0.86274509803921573</v>
+      </c>
+      <c r="C13" s="10">
+        <f>Data!AE13/255*2.56</f>
+        <v>1.1785251826220684</v>
+      </c>
+      <c r="D13" s="10">
+        <f>Data!L13/255*2</f>
+        <v>1.1117262591311035</v>
+      </c>
+      <c r="E13" s="10">
+        <f>Data!L13/255*2*1.56</f>
+        <v>1.7342929642445215</v>
+      </c>
+      <c r="F13" s="10">
+        <f>Data!L13/255*2*1.18</f>
+        <v>1.3118369857747021</v>
+      </c>
+      <c r="G13" s="10">
+        <f>Data!L13/255*2*1.38</f>
+        <v>1.5341822376009226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <f>Data!A14/255</f>
+        <v>0.47058823529411764</v>
+      </c>
+      <c r="B14" s="10">
+        <f>Data!AD14/255*2</f>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="C14" s="10">
+        <f>Data!AE14/255*2.56</f>
+        <v>1.2737993079584775</v>
+      </c>
+      <c r="D14" s="10">
+        <f>Data!L14/255*2</f>
+        <v>1.1700115340253749</v>
+      </c>
+      <c r="E14" s="10">
+        <f>Data!L14/255*2*1.56</f>
+        <v>1.8252179930795849</v>
+      </c>
+      <c r="F14" s="10">
+        <f>Data!L14/255*2*1.18</f>
+        <v>1.3806136101499424</v>
+      </c>
+      <c r="G14" s="10">
+        <f>Data!L14/255*2*1.38</f>
+        <v>1.6146159169550174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <f>Data!A15/255</f>
+        <v>0.50980392156862742</v>
+      </c>
+      <c r="B15" s="10">
+        <f>Data!AD15/255*2</f>
+        <v>1.0196078431372548</v>
+      </c>
+      <c r="C15" s="10">
+        <f>Data!AE15/255*2.56</f>
+        <v>1.3690734332948866</v>
+      </c>
+      <c r="D15" s="10">
+        <f>Data!L15/255*2</f>
+        <v>1.2282968089196462</v>
+      </c>
+      <c r="E15" s="10">
+        <f>Data!L15/255*2*1.56</f>
+        <v>1.9161430219146482</v>
+      </c>
+      <c r="F15" s="10">
+        <f>Data!L15/255*2*1.18</f>
+        <v>1.4493902345251823</v>
+      </c>
+      <c r="G15" s="10">
+        <f>Data!L15/255*2*1.38</f>
+        <v>1.6950495963091117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <f>Data!A16/255</f>
+        <v>0.5490196078431373</v>
+      </c>
+      <c r="B16" s="10">
+        <f>Data!AD16/255*2</f>
+        <v>1.0980392156862746</v>
+      </c>
+      <c r="C16" s="10">
+        <f>Data!AE16/255*2.56</f>
+        <v>1.4643475586312955</v>
+      </c>
+      <c r="D16" s="10">
+        <f>Data!L16/255*2</f>
+        <v>1.2865820838139179</v>
+      </c>
+      <c r="E16" s="10">
+        <f>Data!L16/255*2*1.56</f>
+        <v>2.0070680507497118</v>
+      </c>
+      <c r="F16" s="10">
+        <f>Data!L16/255*2*1.18</f>
+        <v>1.5181668589004231</v>
+      </c>
+      <c r="G16" s="10">
+        <f>Data!L16/255*2*1.38</f>
+        <v>1.7754832756632066</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <f>Data!A17/255</f>
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="B17" s="10">
+        <f>Data!AD17/255*2</f>
+        <v>1.1764705882352942</v>
+      </c>
+      <c r="C17" s="10">
+        <f>Data!AE17/255*2.56</f>
+        <v>1.5596216839677046</v>
+      </c>
+      <c r="D17" s="10">
+        <f>Data!L17/255*2</f>
+        <v>1.344867358708189</v>
+      </c>
+      <c r="E17" s="10">
+        <f>Data!L17/255*2*1.56</f>
+        <v>2.097993079584775</v>
+      </c>
+      <c r="F17" s="10">
+        <f>Data!L17/255*2*1.18</f>
+        <v>1.5869434832756628</v>
+      </c>
+      <c r="G17" s="10">
+        <f>Data!L17/255*2*1.38</f>
+        <v>1.8559169550173007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <f>Data!A18/255</f>
+        <v>0.62745098039215685</v>
+      </c>
+      <c r="B18" s="10">
+        <f>Data!AD18/255*2</f>
+        <v>1.2549019607843137</v>
+      </c>
+      <c r="C18" s="10">
+        <f>Data!AE18/255*2.56</f>
+        <v>1.654895809304114</v>
+      </c>
+      <c r="D18" s="10">
+        <f>Data!L18/255*2</f>
+        <v>1.4031526336024607</v>
+      </c>
+      <c r="E18" s="10">
+        <f>Data!L18/255*2*1.56</f>
+        <v>2.1889181084198386</v>
+      </c>
+      <c r="F18" s="10">
+        <f>Data!L18/255*2*1.18</f>
+        <v>1.6557201076509036</v>
+      </c>
+      <c r="G18" s="10">
+        <f>Data!L18/255*2*1.38</f>
+        <v>1.9363506343713957</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <f>Data!A19/255</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B19" s="10">
+        <f>Data!AD19/255*2</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="C19" s="10">
+        <f>Data!AE19/255*2.56</f>
+        <v>1.7501699346405226</v>
+      </c>
+      <c r="D19" s="10">
+        <f>Data!L19/255*2</f>
+        <v>1.4614379084967322</v>
+      </c>
+      <c r="E19" s="10">
+        <f>Data!L19/255*2*1.56</f>
+        <v>2.2798431372549022</v>
+      </c>
+      <c r="F19" s="10">
+        <f>Data!L19/255*2*1.18</f>
+        <v>1.724496732026144</v>
+      </c>
+      <c r="G19" s="10">
+        <f>Data!L19/255*2*1.38</f>
+        <v>2.0167843137254904</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <f>Data!A20/255</f>
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="B20" s="10">
+        <f>Data!AD20/255*2</f>
+        <v>1.411764705882353</v>
+      </c>
+      <c r="C20" s="10">
+        <f>Data!AE20/255*2.56</f>
+        <v>1.8454440599769319</v>
+      </c>
+      <c r="D20" s="10">
+        <f>Data!L20/255*2</f>
+        <v>1.5197231833910034</v>
+      </c>
+      <c r="E20" s="10">
+        <f>Data!L20/255*2*1.56</f>
+        <v>2.3707681660899653</v>
+      </c>
+      <c r="F20" s="10">
+        <f>Data!L20/255*2*1.18</f>
+        <v>1.7932733564013839</v>
+      </c>
+      <c r="G20" s="10">
+        <f>Data!L20/255*2*1.38</f>
+        <v>2.0972179930795845</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <f>Data!A21/255</f>
+        <v>0.74509803921568629</v>
+      </c>
+      <c r="B21" s="10">
+        <f>Data!AD21/255*2</f>
+        <v>1.4901960784313726</v>
+      </c>
+      <c r="C21" s="10">
+        <f>Data!AE21/255*2.56</f>
+        <v>1.9407181853133408</v>
+      </c>
+      <c r="D21" s="10">
+        <f>Data!L21/255*2</f>
+        <v>1.5780084582852749</v>
+      </c>
+      <c r="E21" s="10">
+        <f>Data!L21/255*2*1.56</f>
+        <v>2.4616931949250289</v>
+      </c>
+      <c r="F21" s="10">
+        <f>Data!L21/255*2*1.18</f>
+        <v>1.8620499807766242</v>
+      </c>
+      <c r="G21" s="10">
+        <f>Data!L21/255*2*1.38</f>
+        <v>2.1776516724336794</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <f>Data!A22/255</f>
+        <v>0.78431372549019607</v>
+      </c>
+      <c r="B22" s="10">
+        <f>Data!AD22/255*2</f>
+        <v>1.5686274509803921</v>
+      </c>
+      <c r="C22" s="10">
+        <f>Data!AE22/255*2.56</f>
+        <v>2.0359923106497497</v>
+      </c>
+      <c r="D22" s="10">
+        <f>Data!L22/255*2</f>
+        <v>1.6362937331795464</v>
+      </c>
+      <c r="E22" s="10">
+        <f>Data!L22/255*2*1.56</f>
+        <v>2.5526182237600925</v>
+      </c>
+      <c r="F22" s="10">
+        <f>Data!L22/255*2*1.18</f>
+        <v>1.9308266051518646</v>
+      </c>
+      <c r="G22" s="10">
+        <f>Data!L22/255*2*1.38</f>
+        <v>2.2580853517877739</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <f>Data!A23/255</f>
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="B23" s="10">
+        <f>Data!AD23/255*2</f>
+        <v>1.6470588235294117</v>
+      </c>
+      <c r="C23" s="10">
+        <f>Data!AE23/255*2.56</f>
+        <v>2.1312664359861593</v>
+      </c>
+      <c r="D23" s="10">
+        <f>Data!L23/255*2</f>
+        <v>1.7024221453287198</v>
+      </c>
+      <c r="E23" s="10">
+        <f>Data!L23/255*2*1.56</f>
+        <v>2.6557785467128032</v>
+      </c>
+      <c r="F23" s="10">
+        <f>Data!L23/255*2*1.18</f>
+        <v>2.0088581314878895</v>
+      </c>
+      <c r="G23" s="10">
+        <f>Data!L23/255*2*1.38</f>
+        <v>2.3493425605536333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <f>Data!A24/255</f>
+        <v>0.86274509803921573</v>
+      </c>
+      <c r="B24" s="10">
+        <f>Data!AD24/255*2</f>
+        <v>1.7254901960784315</v>
+      </c>
+      <c r="C24" s="10">
+        <f>Data!AE24/255*2.56</f>
+        <v>2.2265405613225684</v>
+      </c>
+      <c r="D24" s="10">
+        <f>Data!L24/255*2</f>
+        <v>1.7685505574778932</v>
+      </c>
+      <c r="E24" s="10">
+        <f>Data!L24/255*2*1.56</f>
+        <v>2.7589388696655135</v>
+      </c>
+      <c r="F24" s="10">
+        <f>Data!L24/255*2*1.18</f>
+        <v>2.0868896578239138</v>
+      </c>
+      <c r="G24" s="10">
+        <f>Data!L24/255*2*1.38</f>
+        <v>2.4405997693194923</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <f>Data!A25/255</f>
+        <v>0.90196078431372551</v>
+      </c>
+      <c r="B25" s="10">
+        <f>Data!AD25/255*2</f>
+        <v>1.803921568627451</v>
+      </c>
+      <c r="C25" s="10">
+        <f>Data!AE25/255*2.56</f>
+        <v>2.3218146866589771</v>
+      </c>
+      <c r="D25" s="10">
+        <f>Data!L25/255*2</f>
+        <v>1.8346789696270667</v>
+      </c>
+      <c r="E25" s="10">
+        <f>Data!L25/255*2*1.56</f>
+        <v>2.8620991926182242</v>
+      </c>
+      <c r="F25" s="10">
+        <f>Data!L25/255*2*1.18</f>
+        <v>2.1649211841599385</v>
+      </c>
+      <c r="G25" s="10">
+        <f>Data!L25/255*2*1.38</f>
+        <v>2.5318569780853517</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <f>Data!A26/255</f>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="B26" s="10">
+        <f>Data!AD26/255*2</f>
+        <v>1.8823529411764706</v>
+      </c>
+      <c r="C26" s="10">
+        <f>Data!AE26/255*2.56</f>
+        <v>2.4170888119953866</v>
+      </c>
+      <c r="D26" s="10">
+        <f>Data!L26/255*2</f>
+        <v>1.9008073817762399</v>
+      </c>
+      <c r="E26" s="10">
+        <f>Data!L26/255*2*1.56</f>
+        <v>2.9652595155709345</v>
+      </c>
+      <c r="F26" s="10">
+        <f>Data!L26/255*2*1.18</f>
+        <v>2.2429527104959628</v>
+      </c>
+      <c r="G26" s="10">
+        <f>Data!L26/255*2*1.38</f>
+        <v>2.6231141868512107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <f>Data!A27/255</f>
+        <v>0.98039215686274506</v>
+      </c>
+      <c r="B27" s="10">
+        <f>Data!AD27/255*2</f>
+        <v>1.9607843137254901</v>
+      </c>
+      <c r="C27" s="10">
+        <f>Data!AE27/255*2.56</f>
+        <v>2.5123629373317953</v>
+      </c>
+      <c r="D27" s="10">
+        <f>Data!L27/255*2</f>
+        <v>1.9669357939254133</v>
+      </c>
+      <c r="E27" s="10">
+        <f>Data!L27/255*2*1.56</f>
+        <v>3.0684198385236447</v>
+      </c>
+      <c r="F27" s="10">
+        <f>Data!L27/255*2*1.18</f>
+        <v>2.3209842368319875</v>
+      </c>
+      <c r="G27" s="10">
+        <f>Data!L27/255*2*1.38</f>
+        <v>2.7143713956170701</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <f>Data!A28/255</f>
+        <v>1</v>
+      </c>
+      <c r="B28" s="10">
+        <f>Data!AD28/255*2</f>
+        <v>2</v>
+      </c>
+      <c r="C28" s="10">
+        <f>Data!AE28/255*2.56</f>
+        <v>2.56</v>
+      </c>
+      <c r="D28" s="10">
+        <f>Data!L28/255*2</f>
+        <v>2</v>
+      </c>
+      <c r="E28" s="10">
+        <f>Data!L28/255*2*1.56</f>
+        <v>3.12</v>
+      </c>
+      <c r="F28" s="10">
+        <f>Data!L28/255*2*1.18</f>
+        <v>2.36</v>
+      </c>
+      <c r="G28" s="10">
+        <f>Data!L28/255*2*1.38</f>
+        <v>2.76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bug fix and cleanup
</commit_message>
<xml_diff>
--- a/docs/Calibration_test.xlsx
+++ b/docs/Calibration_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="9345" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="9345" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -3481,11 +3481,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="83517824"/>
-        <c:axId val="83519360"/>
+        <c:axId val="82867328"/>
+        <c:axId val="82868864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83517824"/>
+        <c:axId val="82867328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260"/>
@@ -3499,12 +3499,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83519360"/>
+        <c:crossAx val="82868864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83519360"/>
+        <c:axId val="82868864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3516,14 +3516,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83517824"/>
+        <c:crossAx val="82867328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5775,11 +5774,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="83615104"/>
-        <c:axId val="83620992"/>
+        <c:axId val="82973056"/>
+        <c:axId val="82974592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83615104"/>
+        <c:axId val="82973056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260"/>
@@ -5793,12 +5792,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83620992"/>
+        <c:crossAx val="82974592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83620992"/>
+        <c:axId val="82974592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5810,14 +5809,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83615104"/>
+        <c:crossAx val="82973056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6104,11 +6102,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84821888"/>
-        <c:axId val="84836352"/>
+        <c:axId val="83389056"/>
+        <c:axId val="83391232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84821888"/>
+        <c:axId val="83389056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6165,12 +6163,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84836352"/>
+        <c:crossAx val="83391232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84836352"/>
+        <c:axId val="83391232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6227,7 +6225,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84821888"/>
+        <c:crossAx val="83389056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6883,11 +6881,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="38617472"/>
-        <c:axId val="38570624"/>
+        <c:axId val="83559936"/>
+        <c:axId val="83561856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="38617472"/>
+        <c:axId val="83559936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6895,11 +6893,26 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -6910,13 +6923,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38570624"/>
+        <c:crossAx val="83561856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="38570624"/>
+        <c:axId val="83561856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="140"/>
@@ -6924,11 +6937,26 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -6939,7 +6967,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38617472"/>
+        <c:crossAx val="83559936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7461,11 +7489,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="74273152"/>
-        <c:axId val="74275072"/>
+        <c:axId val="85203968"/>
+        <c:axId val="85230336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74273152"/>
+        <c:axId val="85203968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7473,11 +7501,26 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -7488,13 +7531,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74275072"/>
+        <c:crossAx val="85230336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74275072"/>
+        <c:axId val="85230336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3"/>
@@ -7502,11 +7545,26 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -7517,7 +7575,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74273152"/>
+        <c:crossAx val="85203968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8439,11 +8497,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="73872896"/>
-        <c:axId val="73874432"/>
+        <c:axId val="85015936"/>
+        <c:axId val="85017728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73872896"/>
+        <c:axId val="85015936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -8451,11 +8509,26 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -8466,13 +8539,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73874432"/>
+        <c:crossAx val="85017728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73874432"/>
+        <c:axId val="85017728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.5"/>
@@ -8480,11 +8553,26 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -8495,7 +8583,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73872896"/>
+        <c:crossAx val="85015936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14973,8 +15061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15422,8 +15510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="V2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AL21" sqref="AL21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix calibration for low power rotation
</commit_message>
<xml_diff>
--- a/docs/Calibration_test.xlsx
+++ b/docs/Calibration_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="9345" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="9345" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
     <sheet name="FIgure1" sheetId="7" r:id="rId6"/>
     <sheet name="Figure2" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -3481,11 +3482,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="82867328"/>
-        <c:axId val="82868864"/>
+        <c:axId val="79775232"/>
+        <c:axId val="79776768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82867328"/>
+        <c:axId val="79775232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260"/>
@@ -3499,12 +3500,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82868864"/>
+        <c:crossAx val="79776768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82868864"/>
+        <c:axId val="79776768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3516,13 +3517,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82867328"/>
+        <c:crossAx val="79775232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5774,11 +5776,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="82973056"/>
-        <c:axId val="82974592"/>
+        <c:axId val="79893248"/>
+        <c:axId val="79894784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82973056"/>
+        <c:axId val="79893248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260"/>
@@ -5792,12 +5794,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82974592"/>
+        <c:crossAx val="79894784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82974592"/>
+        <c:axId val="79894784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5809,13 +5811,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82973056"/>
+        <c:crossAx val="79893248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6102,11 +6105,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="83389056"/>
-        <c:axId val="83391232"/>
+        <c:axId val="79985664"/>
+        <c:axId val="79987840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83389056"/>
+        <c:axId val="79985664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6163,12 +6166,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83391232"/>
+        <c:crossAx val="79987840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83391232"/>
+        <c:axId val="79987840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6225,7 +6228,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83389056"/>
+        <c:crossAx val="79985664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6881,11 +6884,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="83559936"/>
-        <c:axId val="83561856"/>
+        <c:axId val="80123776"/>
+        <c:axId val="80134144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83559936"/>
+        <c:axId val="80123776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6923,13 +6926,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83561856"/>
+        <c:crossAx val="80134144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83561856"/>
+        <c:axId val="80134144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="140"/>
@@ -6967,7 +6970,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83559936"/>
+        <c:crossAx val="80123776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7489,11 +7492,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85203968"/>
-        <c:axId val="85230336"/>
+        <c:axId val="83762560"/>
+        <c:axId val="83784832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85203968"/>
+        <c:axId val="83762560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7531,13 +7534,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85230336"/>
+        <c:crossAx val="83784832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85230336"/>
+        <c:axId val="83784832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3"/>
@@ -7575,7 +7578,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85203968"/>
+        <c:crossAx val="83762560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8497,11 +8500,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85015936"/>
-        <c:axId val="85017728"/>
+        <c:axId val="83824640"/>
+        <c:axId val="83826176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85015936"/>
+        <c:axId val="83824640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -8539,13 +8542,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85017728"/>
+        <c:crossAx val="83826176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85017728"/>
+        <c:axId val="83826176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.5"/>
@@ -8583,7 +8586,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85015936"/>
+        <c:crossAx val="83824640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8668,6 +8671,483 @@
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.869884955969289E-2"/>
+          <c:y val="1.1895749873371091E-2"/>
+          <c:w val="0.82960001962371521"/>
+          <c:h val="0.92952402879464624"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Rotation</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$1:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42.107843137254903</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44.215686274509807</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46.32352941176471</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48.431372549019606</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58.03921568627451</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>67.64705882352942</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77.254901960784309</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>86.862745098039213</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>96.470588235294116</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>106.07843137254902</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>115.68627450980392</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>125.29411764705883</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>134.90196078431373</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>144.50980392156862</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>154.11764705882354</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>163.72549019607843</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>173.33333333333334</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>182.94117647058823</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>192.54901960784315</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>202.15686274509804</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>211.76470588235296</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>221.37254901960785</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230.98039215686276</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240.58823529411765</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250.19607843137257</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Curve_old</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$1:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$1:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="69919872"/>
+        <c:axId val="69921408"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="69919872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="260"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69921408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="69921408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69919872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -9445,6 +9925,43 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>428626</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9736,7 +10253,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N1" sqref="N1"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15061,7 +15578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="D7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
@@ -16350,4 +16867,349 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10">
+        <f t="shared" ref="B1:B3" si="0">(A1*(1-10/255) + 10)+(1-A1/40)*30</f>
+        <v>40</v>
+      </c>
+      <c r="C1">
+        <f>A1*(50-20)/50 + 20</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>10</v>
+      </c>
+      <c r="B2" s="10">
+        <f t="shared" si="0"/>
+        <v>42.107843137254903</v>
+      </c>
+      <c r="C2" s="10">
+        <f t="shared" ref="C2:C5" si="1">A2*(50-20)/50 + 20</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>20</v>
+      </c>
+      <c r="B3" s="10">
+        <f t="shared" si="0"/>
+        <v>44.215686274509807</v>
+      </c>
+      <c r="C3" s="10">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>30</v>
+      </c>
+      <c r="B4" s="10">
+        <f>(A4*(1-10/255) + 10)+(1-A4/40)*30</f>
+        <v>46.32352941176471</v>
+      </c>
+      <c r="C4" s="10">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>40</v>
+      </c>
+      <c r="B5" s="10">
+        <f>(A5*(1-10/255) + 10)+(1-A5/40)*30</f>
+        <v>48.431372549019606</v>
+      </c>
+      <c r="C5" s="10">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>50</v>
+      </c>
+      <c r="B6" s="10">
+        <f t="shared" ref="B1:B27" si="2">A6*(1-10/255) + 10</f>
+        <v>58.03921568627451</v>
+      </c>
+      <c r="C6" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>60</v>
+      </c>
+      <c r="B7" s="10">
+        <f t="shared" si="2"/>
+        <v>67.64705882352942</v>
+      </c>
+      <c r="C7" s="7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>70</v>
+      </c>
+      <c r="B8" s="10">
+        <f t="shared" si="2"/>
+        <v>77.254901960784309</v>
+      </c>
+      <c r="C8" s="7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>80</v>
+      </c>
+      <c r="B9" s="10">
+        <f t="shared" si="2"/>
+        <v>86.862745098039213</v>
+      </c>
+      <c r="C9" s="7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>90</v>
+      </c>
+      <c r="B10" s="10">
+        <f t="shared" si="2"/>
+        <v>96.470588235294116</v>
+      </c>
+      <c r="C10" s="7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>100</v>
+      </c>
+      <c r="B11" s="10">
+        <f t="shared" si="2"/>
+        <v>106.07843137254902</v>
+      </c>
+      <c r="C11" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>110</v>
+      </c>
+      <c r="B12" s="10">
+        <f t="shared" si="2"/>
+        <v>115.68627450980392</v>
+      </c>
+      <c r="C12" s="7">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>120</v>
+      </c>
+      <c r="B13" s="10">
+        <f t="shared" si="2"/>
+        <v>125.29411764705883</v>
+      </c>
+      <c r="C13" s="7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>130</v>
+      </c>
+      <c r="B14" s="10">
+        <f t="shared" si="2"/>
+        <v>134.90196078431373</v>
+      </c>
+      <c r="C14" s="7">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>140</v>
+      </c>
+      <c r="B15" s="10">
+        <f t="shared" si="2"/>
+        <v>144.50980392156862</v>
+      </c>
+      <c r="C15" s="7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>150</v>
+      </c>
+      <c r="B16" s="10">
+        <f t="shared" si="2"/>
+        <v>154.11764705882354</v>
+      </c>
+      <c r="C16" s="7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>160</v>
+      </c>
+      <c r="B17" s="10">
+        <f t="shared" si="2"/>
+        <v>163.72549019607843</v>
+      </c>
+      <c r="C17" s="7">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>170</v>
+      </c>
+      <c r="B18" s="10">
+        <f t="shared" si="2"/>
+        <v>173.33333333333334</v>
+      </c>
+      <c r="C18" s="7">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>180</v>
+      </c>
+      <c r="B19" s="10">
+        <f t="shared" si="2"/>
+        <v>182.94117647058823</v>
+      </c>
+      <c r="C19" s="7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>190</v>
+      </c>
+      <c r="B20" s="10">
+        <f t="shared" si="2"/>
+        <v>192.54901960784315</v>
+      </c>
+      <c r="C20" s="7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>200</v>
+      </c>
+      <c r="B21" s="10">
+        <f t="shared" si="2"/>
+        <v>202.15686274509804</v>
+      </c>
+      <c r="C21" s="7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>210</v>
+      </c>
+      <c r="B22" s="10">
+        <f t="shared" si="2"/>
+        <v>211.76470588235296</v>
+      </c>
+      <c r="C22" s="7">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>220</v>
+      </c>
+      <c r="B23" s="10">
+        <f t="shared" si="2"/>
+        <v>221.37254901960785</v>
+      </c>
+      <c r="C23" s="7">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>230</v>
+      </c>
+      <c r="B24" s="10">
+        <f t="shared" si="2"/>
+        <v>230.98039215686276</v>
+      </c>
+      <c r="C24" s="7">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>240</v>
+      </c>
+      <c r="B25" s="10">
+        <f t="shared" si="2"/>
+        <v>240.58823529411765</v>
+      </c>
+      <c r="C25" s="7">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>250</v>
+      </c>
+      <c r="B26" s="10">
+        <f t="shared" si="2"/>
+        <v>250.19607843137257</v>
+      </c>
+      <c r="C26" s="7">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>255</v>
+      </c>
+      <c r="B27" s="10">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="C27" s="7">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>